<commit_message>
support rich text in cells: at some point we might want to stop using our fork and switch over to this module: https://www.npmjs.com/package/xlsx
which replaced the guts of what we forked from.  Unfortunately we'd have to fork that module and re-add support for google docs
</commit_message>
<xml_diff>
--- a/test/fixtures/test.xlsx
+++ b/test/fixtures/test.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="1500" yWindow="560" windowWidth="20300" windowHeight="9960"/>
   </bookViews>
   <sheets>
     <sheet name="hello" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>A1</t>
   </si>
@@ -26,18 +31,56 @@
   </si>
   <si>
     <t>B2</t>
+  </si>
+  <si>
+    <t>C1 &lt; C2 &gt; C1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no format </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bold format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> no format</t>
+    </r>
+  </si>
+  <si>
+    <t>D1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -364,29 +407,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>